<commit_message>
Restructure of child Covid surveys plus additional Geographic datasets
</commit_message>
<xml_diff>
--- a/docs/csv/BiBBS__full_data_dictionary.xlsx
+++ b/docs/csv/BiBBS__full_data_dictionary.xlsx
@@ -8,12 +8,13 @@
   <sheets>
     <sheet name="BiBBS_Baseline" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="BiBBS_CohortInfo" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="BiBBS_Geographic" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="1255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="1316">
   <si>
     <t xml:space="preserve">project</t>
   </si>
@@ -3784,6 +3785,189 @@
   </si>
   <si>
     <t xml:space="preserve">BiBBS_CohortInfo.partner.n_pregnancies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ch_core_geog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_address_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.date_address_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of latest available address data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.age_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Participants actual age (months)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_closest_data_point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.age_closest_data_point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age at data point closest to participants actual age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temporal_accuracy_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.temporal_accuracy_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difference in months between participants age at closest data point and actual a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSOA11CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.LSOA11CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSOA 2011 code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WD21CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.WD21CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ward 2021 code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_in_bfd_la</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.is_in_bfd_la</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is participant in Bradford LA?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is_in_bibbs_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.is_in_bibbs_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is participant in BiBBS area?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.data_source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source of data: registration (1) or tracing (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration|Tracing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is participant in BiB (1) or BiBBS (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiB|BiBBS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not_in_eng_wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.not_in_eng_wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates if address is not in England or Wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing_address_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.missing_address_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates if record has missing address data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poor_qual_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ch_core_geog.poor_qual_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicates if record has poor quality data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house_nbhd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.house_nbhd.age_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD_2010_decile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.house_nbhd.IMD_2010_decile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD 2010 decile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD_2010_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.house_nbhd.IMD_2010_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD 2010 score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD_2019_decile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.house_nbhd.IMD_2019_decile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD 2019 decile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD_2019_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.house_nbhd.IMD_2019_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMD 2019 score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">house_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.house_nbhd.house_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terraced|Semi-Detached|Self Contained Flat (Includes Maisonette / Apartment)|Detached|Other</t>
   </si>
 </sst>
 </file>
@@ -3851,6 +4035,24 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I57" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:I57"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="project"/>
+    <tableColumn id="2" name="table"/>
+    <tableColumn id="3" name="variable"/>
+    <tableColumn id="4" name="full_name"/>
+    <tableColumn id="5" name="label"/>
+    <tableColumn id="6" name="value_type"/>
+    <tableColumn id="7" name="description"/>
+    <tableColumn id="8" name="categories"/>
+    <tableColumn id="9" name="categories_label"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I20" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I20"/>
   <tableColumns count="9">
     <tableColumn id="1" name="project"/>
     <tableColumn id="2" name="table"/>
@@ -14398,4 +14600,621 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <cols>
+    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="12.71" hidden="0" customWidth="1"/>
+    <col min="3" max="3" width="22.71" hidden="0" customWidth="1"/>
+    <col min="4" max="4" width="52.71" hidden="0" customWidth="1"/>
+    <col min="5" max="5" width="80.71" hidden="0" customWidth="1"/>
+    <col min="6" max="6" width="10.71" hidden="0" customWidth="1"/>
+    <col min="7" max="7" width="11.71" hidden="0" customWidth="1"/>
+    <col min="8" max="8" width="10.71" hidden="0" customWidth="1"/>
+    <col min="9" max="9" width="91.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="9.15" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="9.15" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="9.15" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="9.15" hidden="0" customWidth="1"/>
+    <col min="14" max="14" width="9.15" hidden="0" customWidth="1"/>
+    <col min="15" max="15" width="9.15" hidden="0" customWidth="1"/>
+    <col min="16" max="16" width="9.15" hidden="0" customWidth="1"/>
+    <col min="17" max="17" width="9.15" hidden="0" customWidth="1"/>
+    <col min="18" max="18" width="9.15" hidden="0" customWidth="1"/>
+    <col min="19" max="19" width="9.15" hidden="0" customWidth="1"/>
+    <col min="20" max="20" width="9.15" hidden="0" customWidth="1"/>
+    <col min="21" max="21" width="9.15" hidden="0" customWidth="1"/>
+    <col min="22" max="22" width="9.15" hidden="0" customWidth="1"/>
+    <col min="23" max="23" width="9.15" hidden="0" customWidth="1"/>
+    <col min="24" max="24" width="9.15" hidden="0" customWidth="1"/>
+    <col min="25" max="25" width="9.15" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="9.15" hidden="0" customWidth="1"/>
+    <col min="27" max="27" width="9.15" hidden="0" customWidth="1"/>
+    <col min="28" max="28" width="9.15" hidden="0" customWidth="1"/>
+    <col min="29" max="29" width="9.15" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="9.15" hidden="0" customWidth="1"/>
+    <col min="31" max="31" width="9.15" hidden="0" customWidth="1"/>
+    <col min="32" max="32" width="9.15" hidden="0" customWidth="1"/>
+    <col min="33" max="33" width="9.15" hidden="0" customWidth="1"/>
+    <col min="34" max="34" width="9.15" hidden="0" customWidth="1"/>
+    <col min="35" max="35" width="9.15" hidden="0" customWidth="1"/>
+    <col min="36" max="36" width="9.15" hidden="0" customWidth="1"/>
+    <col min="37" max="37" width="9.15" hidden="0" customWidth="1"/>
+    <col min="38" max="38" width="9.15" hidden="0" customWidth="1"/>
+    <col min="39" max="39" width="9.15" hidden="0" customWidth="1"/>
+    <col min="40" max="40" width="9.15" hidden="0" customWidth="1"/>
+    <col min="41" max="41" width="9.15" hidden="0" customWidth="1"/>
+    <col min="42" max="42" width="9.15" hidden="0" customWidth="1"/>
+    <col min="43" max="43" width="9.15" hidden="0" customWidth="1"/>
+    <col min="44" max="44" width="9.15" hidden="0" customWidth="1"/>
+    <col min="45" max="45" width="9.15" hidden="0" customWidth="1"/>
+    <col min="46" max="46" width="9.15" hidden="0" customWidth="1"/>
+    <col min="47" max="47" width="9.15" hidden="0" customWidth="1"/>
+    <col min="48" max="48" width="9.15" hidden="0" customWidth="1"/>
+    <col min="49" max="49" width="9.15" hidden="0" customWidth="1"/>
+    <col min="50" max="50" width="9.15" hidden="0" customWidth="1"/>
+    <col min="51" max="51" width="9.15" hidden="0" customWidth="1"/>
+    <col min="52" max="52" width="9.15" hidden="0" customWidth="1"/>
+    <col min="53" max="53" width="9.15" hidden="0" customWidth="1"/>
+    <col min="54" max="54" width="9.15" hidden="0" customWidth="1"/>
+    <col min="55" max="55" width="9.15" hidden="0" customWidth="1"/>
+    <col min="56" max="56" width="9.15" hidden="0" customWidth="1"/>
+    <col min="57" max="57" width="9.15" hidden="0" customWidth="1"/>
+    <col min="58" max="58" width="9.15" hidden="0" customWidth="1"/>
+    <col min="59" max="59" width="9.15" hidden="0" customWidth="1"/>
+    <col min="60" max="60" width="9.15" hidden="0" customWidth="1"/>
+    <col min="61" max="61" width="9.15" hidden="0" customWidth="1"/>
+    <col min="62" max="62" width="9.15" hidden="0" customWidth="1"/>
+    <col min="63" max="63" width="9.15" hidden="0" customWidth="1"/>
+    <col min="64" max="64" width="9.15" hidden="0" customWidth="1"/>
+    <col min="65" max="65" width="9.15" hidden="0" customWidth="1"/>
+    <col min="66" max="66" width="9.15" hidden="0" customWidth="1"/>
+    <col min="67" max="67" width="9.15" hidden="0" customWidth="1"/>
+    <col min="68" max="68" width="9.15" hidden="0" customWidth="1"/>
+    <col min="69" max="69" width="9.15" hidden="0" customWidth="1"/>
+    <col min="70" max="70" width="9.15" hidden="0" customWidth="1"/>
+    <col min="71" max="71" width="9.15" hidden="0" customWidth="1"/>
+    <col min="72" max="72" width="9.15" hidden="0" customWidth="1"/>
+    <col min="73" max="73" width="9.15" hidden="0" customWidth="1"/>
+    <col min="74" max="74" width="9.15" hidden="0" customWidth="1"/>
+    <col min="75" max="75" width="9.15" hidden="0" customWidth="1"/>
+    <col min="76" max="76" width="9.15" hidden="0" customWidth="1"/>
+    <col min="77" max="77" width="9.15" hidden="0" customWidth="1"/>
+    <col min="78" max="78" width="9.15" hidden="0" customWidth="1"/>
+    <col min="79" max="79" width="9.15" hidden="0" customWidth="1"/>
+    <col min="80" max="80" width="9.15" hidden="0" customWidth="1"/>
+    <col min="81" max="81" width="9.15" hidden="0" customWidth="1"/>
+    <col min="82" max="82" width="9.15" hidden="0" customWidth="1"/>
+    <col min="83" max="83" width="9.15" hidden="0" customWidth="1"/>
+    <col min="84" max="84" width="9.15" hidden="0" customWidth="1"/>
+    <col min="85" max="85" width="9.15" hidden="0" customWidth="1"/>
+    <col min="86" max="86" width="9.15" hidden="0" customWidth="1"/>
+    <col min="87" max="87" width="9.15" hidden="0" customWidth="1"/>
+    <col min="88" max="88" width="9.15" hidden="0" customWidth="1"/>
+    <col min="89" max="89" width="9.15" hidden="0" customWidth="1"/>
+    <col min="90" max="90" width="9.15" hidden="0" customWidth="1"/>
+    <col min="91" max="91" width="9.15" hidden="0" customWidth="1"/>
+    <col min="92" max="92" width="9.15" hidden="0" customWidth="1"/>
+    <col min="93" max="93" width="9.15" hidden="0" customWidth="1"/>
+    <col min="94" max="94" width="9.15" hidden="0" customWidth="1"/>
+    <col min="95" max="95" width="9.15" hidden="0" customWidth="1"/>
+    <col min="96" max="96" width="9.15" hidden="0" customWidth="1"/>
+    <col min="97" max="97" width="9.15" hidden="0" customWidth="1"/>
+    <col min="98" max="98" width="9.15" hidden="0" customWidth="1"/>
+    <col min="99" max="99" width="9.15" hidden="0" customWidth="1"/>
+    <col min="100" max="100" width="9.15" hidden="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1264</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1265</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1267</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1268</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1270</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1271</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1273</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1276</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1279</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1282</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1283</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1286</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1287</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1293</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1296</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1299</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1300</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1301</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1302</v>
+      </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1305</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1311</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20" t="s">
+        <v>81</v>
+      </c>
+      <c r="I20" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Some additional BiB baseline tables
</commit_message>
<xml_diff>
--- a/docs/csv/BiBBS__full_data_dictionary.xlsx
+++ b/docs/csv/BiBBS__full_data_dictionary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="1316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1330" uniqueCount="1330">
   <si>
     <t xml:space="preserve">project</t>
   </si>
@@ -3914,6 +3914,48 @@
   </si>
   <si>
     <t xml:space="preserve">Indicates if record has poor quality data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ad_core_geog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.date_address_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.age_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.age_closest_data_point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.temporal_accuracy_m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.LSOA11CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.WD21CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.is_in_bfd_la</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.is_in_bibbs_area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.data_source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.not_in_eng_wales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.missing_address_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BiBBS_Geographic.ad_core_geog.poor_qual_data</t>
   </si>
   <si>
     <t xml:space="preserve">house_nbhd</t>
@@ -3973,7 +4015,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -4051,8 +4093,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I20" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:I20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:I33" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I33"/>
   <tableColumns count="9">
     <tableColumn id="1" name="project"/>
     <tableColumn id="2" name="table"/>
@@ -4346,10 +4388,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -13155,10 +13197,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -14603,10 +14645,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
@@ -15076,16 +15118,16 @@
         <v>1298</v>
       </c>
       <c r="C15" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="D15" t="s">
         <v>1299</v>
       </c>
       <c r="E15" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
@@ -15099,13 +15141,13 @@
         <v>1298</v>
       </c>
       <c r="C16" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D16" t="s">
         <v>1300</v>
       </c>
-      <c r="D16" t="s">
-        <v>1301</v>
-      </c>
       <c r="E16" t="s">
-        <v>1302</v>
+        <v>1262</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -15122,13 +15164,13 @@
         <v>1298</v>
       </c>
       <c r="C17" t="s">
-        <v>1303</v>
+        <v>1263</v>
       </c>
       <c r="D17" t="s">
-        <v>1304</v>
+        <v>1301</v>
       </c>
       <c r="E17" t="s">
-        <v>1305</v>
+        <v>1265</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
@@ -15145,13 +15187,13 @@
         <v>1298</v>
       </c>
       <c r="C18" t="s">
-        <v>1306</v>
+        <v>1266</v>
       </c>
       <c r="D18" t="s">
-        <v>1307</v>
+        <v>1302</v>
       </c>
       <c r="E18" t="s">
-        <v>1308</v>
+        <v>1268</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -15168,16 +15210,16 @@
         <v>1298</v>
       </c>
       <c r="C19" t="s">
-        <v>1309</v>
+        <v>1269</v>
       </c>
       <c r="D19" t="s">
-        <v>1310</v>
+        <v>1303</v>
       </c>
       <c r="E19" t="s">
-        <v>1311</v>
+        <v>1271</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
@@ -15191,23 +15233,350 @@
         <v>1298</v>
       </c>
       <c r="C20" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1304</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1275</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1277</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21"/>
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1278</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1283</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1285</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1308</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1287</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1309</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25"/>
+      <c r="H25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1310</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1294</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1311</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27"/>
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B28" t="s">
         <v>1312</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C28" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D28" t="s">
         <v>1313</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E28" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C29" t="s">
         <v>1314</v>
       </c>
-      <c r="F20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20"/>
-      <c r="H20" t="s">
+      <c r="D29" t="s">
+        <v>1315</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1316</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1317</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1318</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1319</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1321</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1322</v>
+      </c>
+      <c r="F31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1324</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1325</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1328</v>
+      </c>
+      <c r="F33" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33" t="s">
         <v>81</v>
       </c>
-      <c r="I20" t="s">
-        <v>1315</v>
+      <c r="I33" t="s">
+        <v>1329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>